<commit_message>
Added support for language tags on string literals
</commit_message>
<xml_diff>
--- a/examples/manufacturers.xlsx
+++ b/examples/manufacturers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqechuc/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqechuc/PycharmProjects/excel2rdf/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA56A24D-2EB5-ED44-A346-7E41918659DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76A3C33-1DA1-6049-A2D2-C1366B06B893}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4020" yWindow="-20540" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>https://w3id.org/tern/ontologies/org/Manufacturer</t>
   </si>
   <si>
-    <t>Aalborg</t>
-  </si>
-  <si>
     <t>Advantech</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>dcterms:modified</t>
+  </si>
+  <si>
+    <t>Aalborg@en</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -605,6 +605,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -923,10 +926,10 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,1633 +957,1633 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
+      <c r="F2" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="11" t="str">
         <f ca="1">TEXT(NOW(),"YYYY-MM-DD"&amp;"T"&amp;"HH:MM:SS")&amp;"+00:00"</f>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J2" s="11" t="str">
         <f t="shared" ref="I2:J53" ca="1" si="0">TEXT(NOW(),"YYYY-MM-DD"&amp;"T"&amp;"HH:MM:SS")&amp;"+00:00"</f>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J3" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J4" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J5" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J6" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J7" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J8" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J9" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J10" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J11" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J12" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J13" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J14" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J15" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J16" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J17" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="H18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="I18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J18" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D19" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J19" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J20" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J21" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="I22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J22" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J23" s="11" t="str">
         <f t="shared" ref="J23:J53" ca="1" si="1">TEXT(NOW(),"YYYY-MM-DD"&amp;"T"&amp;"HH:MM:SS")&amp;"+00:00"</f>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J24" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J25" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D26" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J26" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D27" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J27" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J28" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="I29" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J29" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D30" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I30" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J30" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J31" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J32" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J33" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D34" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J34" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="I35" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J35" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D36" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J36" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J37" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G38" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="I38" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J38" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J39" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J40" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J41" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J42" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J43" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D44" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J44" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D45" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J45" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D46" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J46" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J47" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D48" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J48" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D49" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J49" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D50" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I50" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J50" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D51" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J51" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D52" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J52" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D53" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
       <c r="J53" s="11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>2020-04-01T17:43:13+00:00</v>
+        <v>2020-04-02T12:00:48+00:00</v>
       </c>
     </row>
   </sheetData>
@@ -2606,9 +2609,10 @@
     <hyperlink ref="A17" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="A34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="G50" r:id="rId21" xr:uid="{BB6A1705-6D12-B84B-A7B7-CC161DF69079}"/>
+    <hyperlink ref="F2" r:id="rId22" xr:uid="{DC04A2C9-916D-BA42-8042-08376D8AA2A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2624,65 +2628,65 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
         <v>133</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>